<commit_message>
Atualizando envio de datas
</commit_message>
<xml_diff>
--- a/codigo/Exemplo.xlsx
+++ b/codigo/Exemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\higor\Desktop\whatspy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\higor\Desktop\whatspy\codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A09D76-94DC-4B4A-9BE1-8A5976936242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27A457B-8D45-45B2-A459-A17BFA0B0FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Contatos</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Shape2</t>
+  </si>
+  <si>
+    <t>Datas</t>
   </si>
 </sst>
 </file>
@@ -78,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,39 +469,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1">
+        <v>44583.75</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44582.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>